<commit_message>
1st/2nd trip as clean format
</commit_message>
<xml_diff>
--- a/templates/print_1st2ndtrip.xlsx
+++ b/templates/print_1st2ndtrip.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlou\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlou\Desktop\billing automation\ltbap\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76050DA2-ADC9-4C9C-B513-6463ED8BB18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C387BB2C-2731-46F3-BE0E-9E80D8647B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t xml:space="preserve">                                 LORKWEN TRUCKING SERVICES</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>STA Ref No.:</t>
-  </si>
-  <si>
-    <t>V4563/LFN1487</t>
   </si>
   <si>
     <t>TRIP TICKET NO.:</t>
@@ -503,29 +500,8 @@
   </cellStyleXfs>
   <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -537,9 +513,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -549,21 +522,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,7 +537,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -600,20 +563,54 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,779 +914,768 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="31.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="3"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="53"/>
     </row>
     <row r="2" spans="1:15" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="50"/>
+      <c r="E2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="57">
         <v>2393</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="G3" s="7" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="G3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="10"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+      <c r="A4" s="1"/>
       <c r="L4" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="11">
-        <v>45918</v>
-      </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="13"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="16" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="14" t="s">
+      <c r="F5" s="50"/>
+      <c r="G5" s="6"/>
+      <c r="I5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="14" t="s">
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="13"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="I6" s="14" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="I6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="13"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="I7" s="14" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="I7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="13"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
+      <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="11"/>
       <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="O8" s="13"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+      <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="I9" s="14" t="s">
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="I9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="13"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="K10" s="22"/>
-      <c r="O10" s="13"/>
+      <c r="A10" s="1"/>
+      <c r="K10" s="11"/>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="24" t="s">
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="10"/>
+      <c r="L11" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="26">
-        <v>139544</v>
-      </c>
-      <c r="L11" s="27" t="s">
+      <c r="M11" s="45"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="15"/>
+      <c r="G12" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="28"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="13"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="30"/>
-      <c r="G12" t="s">
+      <c r="J12" s="6"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="15"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="18"/>
+      <c r="L13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="17">
-        <v>3596</v>
-      </c>
-      <c r="K12" s="31"/>
-      <c r="L12" s="30"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="13"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="33"/>
-      <c r="L13" s="34" t="s">
+      <c r="N13" s="17"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="15"/>
+      <c r="L14" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="N13" s="32"/>
-      <c r="O13" s="13"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="30"/>
-      <c r="L14" s="34" t="s">
+      <c r="N14" s="17"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A15" s="1"/>
+      <c r="B15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="32"/>
-      <c r="O14" s="13"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A15" s="4"/>
-      <c r="B15" s="35" t="s">
+      <c r="J15" t="s">
         <v>34</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" s="21"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="15"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" ht="25.8" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="13"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="30"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="13"/>
-    </row>
-    <row r="17" spans="1:15" ht="25.8" x14ac:dyDescent="0.4">
-      <c r="A17" s="4"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="42">
-        <v>380</v>
-      </c>
-      <c r="D17" s="43" t="s">
+      <c r="L17" s="23"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="15"/>
+      <c r="L18" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="39"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="13"/>
-    </row>
-    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="30"/>
-      <c r="L18" s="44" t="s">
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="31"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="15"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M18" s="45"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="13"/>
-    </row>
-    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="4"/>
-      <c r="B19" s="47"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="13"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="30"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="13"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="13"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="51" t="s">
+      <c r="K22" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="51" t="s">
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="F24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="47"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="K24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="O22" s="13"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="O23" s="13"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="F24" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="53">
-        <v>45918</v>
-      </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="K24" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="13"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="4"/>
     </row>
     <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="54"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="56"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="38"/>
     </row>
     <row r="26" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:15" ht="31.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="3"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="53"/>
     </row>
     <row r="28" spans="1:15" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A28" s="4"/>
-      <c r="B28" s="57" t="s">
+      <c r="A28" s="1"/>
+      <c r="B28" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="E28" s="7" t="s">
+      <c r="C28" s="50"/>
+      <c r="E28" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8" t="s">
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28" s="57">
         <v>2394</v>
       </c>
-      <c r="O28" s="10"/>
+      <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="G29" s="7" t="s">
+      <c r="A29" s="1"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="G29" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="10"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="1"/>
       <c r="L30" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="48">
         <v>45918</v>
       </c>
-      <c r="N30" s="12"/>
-      <c r="O30" s="13"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="1"/>
+      <c r="B31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="16" t="s">
+      <c r="D31" s="43"/>
+      <c r="E31" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="17" t="s">
+      <c r="F31" s="50"/>
+      <c r="G31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K31" s="19"/>
+      <c r="K31" s="9"/>
       <c r="L31" t="s">
         <v>12</v>
       </c>
-      <c r="M31" s="15" t="s">
+      <c r="M31" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="N31" s="12"/>
-      <c r="O31" s="13"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="1"/>
+      <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="I32" s="14" t="s">
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="I32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J32" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="13"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="4"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="1"/>
       <c r="B33" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="I33" s="14" t="s">
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="I33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J33" s="20" t="s">
+      <c r="J33" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="13"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="41"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="1"/>
       <c r="B34" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="11"/>
       <c r="E34" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="O34" s="13"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="O34" s="4"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="1"/>
       <c r="B35" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="I35" s="14" t="s">
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="I35" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="J35" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="13"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="4"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="K36" s="22"/>
-      <c r="O36" s="13"/>
+      <c r="A36" s="1"/>
+      <c r="K36" s="11"/>
+      <c r="O36" s="4"/>
     </row>
     <row r="37" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="23" t="s">
+      <c r="A37" s="1"/>
+      <c r="B37" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="24" t="s">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="10">
+        <v>139536</v>
+      </c>
+      <c r="L37" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="26">
-        <v>139536</v>
-      </c>
-      <c r="L37" s="27" t="s">
+      <c r="M37" s="45"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="15"/>
+      <c r="G38" t="s">
         <v>30</v>
       </c>
-      <c r="M37" s="28"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="13"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="30"/>
-      <c r="G38" t="s">
+      <c r="J38" s="6">
+        <v>71035</v>
+      </c>
+      <c r="K38" s="16"/>
+      <c r="L38" s="15"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="15"/>
+      <c r="L39" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J38" s="17">
-        <v>71035</v>
-      </c>
-      <c r="K38" s="31"/>
-      <c r="L38" s="30"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="13"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
-      <c r="B39" s="30"/>
-      <c r="L39" s="34" t="s">
+      <c r="N39" s="17"/>
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="15"/>
+      <c r="L40" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="N39" s="32"/>
-      <c r="O39" s="13"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="30"/>
-      <c r="L40" s="34" t="s">
+      <c r="N40" s="17"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A41" s="1"/>
+      <c r="B41" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N40" s="32"/>
-      <c r="O40" s="13"/>
-    </row>
-    <row r="41" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A41" s="4"/>
-      <c r="B41" s="35" t="s">
+      <c r="L41" s="21"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="4"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="15"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="4"/>
+    </row>
+    <row r="43" spans="1:15" ht="25.8" x14ac:dyDescent="0.4">
+      <c r="A43" s="1"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26">
+        <v>518</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="L43" s="23"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="4"/>
+    </row>
+    <row r="44" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+      <c r="B44" s="15"/>
+      <c r="C44" t="s">
         <v>34</v>
       </c>
-      <c r="L41" s="36"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="13"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="30"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="13"/>
-    </row>
-    <row r="43" spans="1:15" ht="25.8" x14ac:dyDescent="0.4">
-      <c r="A43" s="4"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="42">
-        <v>518</v>
-      </c>
-      <c r="D43" s="43" t="s">
+      <c r="L44" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="L43" s="39"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="40"/>
-      <c r="O43" s="13"/>
-    </row>
-    <row r="44" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="4"/>
-      <c r="B44" s="30"/>
-      <c r="C44" t="s">
-        <v>35</v>
-      </c>
-      <c r="L44" s="44" t="s">
+      <c r="M44" s="29"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="4"/>
+    </row>
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="A45" s="1"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="34"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="22"/>
+      <c r="O45" s="4"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="15"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="4"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="4"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M44" s="45"/>
-      <c r="N44" s="46"/>
-      <c r="O44" s="13"/>
-    </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="4"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="50"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="37"/>
-      <c r="N45" s="38"/>
-      <c r="O45" s="13"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="30"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="13"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="37"/>
-      <c r="L47" s="37"/>
-      <c r="M47" s="37"/>
-      <c r="N47" s="38"/>
-      <c r="O47" s="13"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
-      <c r="B48" s="51" t="s">
+      <c r="K48" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="K48" s="51" t="s">
+      <c r="O48" s="4"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="O49" s="4"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="F50" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="47">
+        <v>45918</v>
+      </c>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="K50" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="O48" s="13"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
-      <c r="O49" s="13"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="F50" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="53">
-        <v>45918</v>
-      </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="K50" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="L50" s="37"/>
-      <c r="M50" s="37"/>
-      <c r="N50" s="37"/>
-      <c r="O50" s="13"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="4"/>
     </row>
     <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="54"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="55"/>
-      <c r="M51" s="55"/>
-      <c r="N51" s="55"/>
-      <c r="O51" s="56"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="38"/>
     </row>
     <row r="52" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="J35:N35"/>
-    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="A27:O27"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="E28:K28"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="G29:I29"/>
     <mergeCell ref="G50:I50"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="C31:D31"/>
@@ -1697,32 +1683,11 @@
     <mergeCell ref="M31:N31"/>
     <mergeCell ref="C32:G32"/>
     <mergeCell ref="J32:N32"/>
-    <mergeCell ref="A27:O27"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="E28:K28"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="J35:N35"/>
+    <mergeCell ref="L37:N37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>